<commit_message>
Changed the Test Case Sheet. Added Cases for Searching in the Events Page and one for New Events Page. -Hitarth Doctor
</commit_message>
<xml_diff>
--- a/SocialTables_tBlocks Test cases sheet V1.0.xlsx
+++ b/SocialTables_tBlocks Test cases sheet V1.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hitarthdoctor\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hitarthdoctor\Documents\GitHub\KiwiQA-Services-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,12 +26,11 @@
     <definedName name="test">Sheet4!$A$1:$A$4</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="357">
   <si>
     <t>Project Name</t>
   </si>
@@ -1472,9 +1471,6 @@
 5. Click on Name</t>
   </si>
   <si>
-    <t>User should able to see Sorted List by Names and also the Change in th Sort-icon</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">To verify User can Perform Sorting by </t>
     </r>
@@ -1506,9 +1502,6 @@
 5. Click on Date</t>
   </si>
   <si>
-    <t>User should able to see Sorted List by Dates and also the Change in th Sort-icon</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">To verify User can Perform Sorting by </t>
     </r>
@@ -1540,9 +1533,6 @@
 5. Click on Category</t>
   </si>
   <si>
-    <t>User should able to see Sorted List by Catagories and also the Change in th Sort-icon</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">To verify User can Perform Sorting by </t>
     </r>
@@ -1574,9 +1564,6 @@
 5. Click on Location</t>
   </si>
   <si>
-    <t>User should able to see Sorted List by Location and also the Change in th Sort-icon</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">To verify User can Perform Sorting by </t>
     </r>
@@ -1608,33 +1595,6 @@
 5. Click on Owner</t>
   </si>
   <si>
-    <t>User should able to see Sorted List by Owner and also the Change in th Sort-icon</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">To verify User </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">can not </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>have From Date Greater than that of To Date</t>
-    </r>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">To verify User can Perform Sorting by </t>
     </r>
@@ -1701,6 +1661,137 @@
   </si>
   <si>
     <t>TC_PT_59</t>
+  </si>
+  <si>
+    <t>NEW EVENT PAGE</t>
+  </si>
+  <si>
+    <t>1. Open URL (staging.socialtables.com)
+2. Click on LOGIN
+3. Enter correct login Credentials
+4. You should be directed to EVENTS page on successful LOGIN
+5. Click on New Event
+6. Wait for New Event to load</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Correct rendering of the page should be visible to User.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>1. New Event form</t>
+    </r>
+  </si>
+  <si>
+    <t>To verify that the New Event page renders correctly, with the New Event Form</t>
+  </si>
+  <si>
+    <t>1. Open URL (staging.socialtables.com)
+2. Click on LOGIN
+3. Enter correct login Credentials
+4. You should be directed to EVENTS page on successful LOGIN
+5. Select a Owner from the list of Owners</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To verify User </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">can not </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>have From-Date Greater than that of To-Date</t>
+    </r>
+  </si>
+  <si>
+    <t>To verify User can select any Category from the list of Categories to search</t>
+  </si>
+  <si>
+    <t>To verify User can select any Owner from the list of Owners to search</t>
+  </si>
+  <si>
+    <t>1. Open URL (staging.socialtables.com)
+2. Click on LOGIN
+3. Enter correct login Credentials
+4. You should be directed to EVENTS page on successful LOGIN
+5. Select a Owner from the list of Categories</t>
+  </si>
+  <si>
+    <t>User should able to see Sorted List by Names and also the Change in the Sort-icon</t>
+  </si>
+  <si>
+    <t>User should able to see Sorted List by Dates and also the Change in the Sort-icon</t>
+  </si>
+  <si>
+    <t>User should able to see Sorted List by Categories and also the Change in the Sort-icon</t>
+  </si>
+  <si>
+    <t>User should able to see Sorted List by Location and also the Change in the Sort-icon</t>
+  </si>
+  <si>
+    <t>User should able to see Sorted List by Owner and also the Change in the Sort-icon</t>
+  </si>
+  <si>
+    <t>To verify User can select any Owner from the list of Location to search</t>
+  </si>
+  <si>
+    <t>1. Open URL (staging.socialtables.com)
+2. Click on LOGIN
+3. Enter correct login Credentials
+4. You should be directed to EVENTS page on successful LOGIN
+5. Select a Owner from the list of Locations</t>
+  </si>
+  <si>
+    <t>User should be able to Select from such a selection of Lacations and receive appropriate list of events</t>
+  </si>
+  <si>
+    <t>User should be able to Select from such a selection of Categories and receive appropriate list of events</t>
+  </si>
+  <si>
+    <t>User should be able to Select from such a selection of Ownes and receive appropriate list of events</t>
+  </si>
+  <si>
+    <t>To verify User can select any Date from the list of From-Date to search</t>
+  </si>
+  <si>
+    <t>1. Open URL (staging.socialtables.com)
+2. Click on LOGIN
+3. Enter correct login Credentials
+4. You should be directed to EVENTS page on successful LOGIN
+5. Select a Date from the list of From-Date</t>
+  </si>
+  <si>
+    <t>User should be able to Select from such a selection of Dates and receive appropriate list of events</t>
+  </si>
+  <si>
+    <t>1. Open URL (staging.socialtables.com)
+2. Click on LOGIN
+3. Enter correct login Credentials
+4. You should be directed to EVENTS page on successful LOGIN
+5. Select a Date from the list of To-Dates</t>
+  </si>
+  <si>
+    <t>To verify User can select any Date from the list of To-Dates to search</t>
   </si>
 </sst>
 </file>
@@ -2306,6 +2397,11 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2353,11 +2449,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2365,7 +2456,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
-  <dxfs count="88">
+  <dxfs count="104">
     <dxf>
       <font>
         <color rgb="FF38761D"/>
@@ -3201,6 +3292,23 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF38761D"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFCC0000"/>
       </font>
       <fill>
@@ -3218,6 +3326,23 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFB45F06"/>
       </font>
       <fill>
@@ -3235,6 +3360,23 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FFB45F06"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF99"/>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF674EA7"/>
       </font>
       <fill>
@@ -3252,6 +3394,23 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF674EA7"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9D2E9"/>
+          <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF38761D"/>
       </font>
       <fill>
@@ -3320,6 +3479,57 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF38761D"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFB45F06"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF99"/>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF674EA7"/>
       </font>
       <fill>
@@ -3581,6 +3791,159 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFFF99"/>
           <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF674EA7"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9D2E9"/>
+          <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF38761D"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFB45F06"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF99"/>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF674EA7"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9D2E9"/>
+          <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF38761D"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFB45F06"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF99"/>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF674EA7"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9D2E9"/>
+          <bgColor rgb="FFD9D2E9"/>
         </patternFill>
       </fill>
       <border>
@@ -4085,7 +4448,7 @@
                   <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4100,11 +4463,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-955358736"/>
-        <c:axId val="-955345680"/>
+        <c:axId val="-860472448"/>
+        <c:axId val="-860469728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-955358736"/>
+        <c:axId val="-860472448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4129,7 +4492,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-955345680"/>
+        <c:crossAx val="-860469728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -4137,7 +4500,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-955345680"/>
+        <c:axId val="-860469728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4173,7 +4536,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-955358736"/>
+        <c:crossAx val="-860472448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4658,14 +5021,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="45"/>
       <c r="G1" s="1"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -4674,12 +5037,12 @@
       <c r="L1" s="3"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="42"/>
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="45"/>
       <c r="G2" s="1"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -4688,12 +5051,12 @@
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="42"/>
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="45"/>
       <c r="G3" s="1"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -4702,12 +5065,12 @@
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="43"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="44"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="47"/>
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -4719,13 +5082,13 @@
       <c r="A5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
       <c r="G5" s="9"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -4737,13 +5100,13 @@
       <c r="A6" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
       <c r="G6" s="9"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -4755,13 +5118,13 @@
       <c r="A7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
       <c r="G7" s="9"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -4773,13 +5136,13 @@
       <c r="A8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
       <c r="G8" s="9"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -4791,13 +5154,13 @@
       <c r="A9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
       <c r="G9" s="9"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -4809,13 +5172,13 @@
       <c r="A10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
       <c r="G10" s="9"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -4827,13 +5190,13 @@
       <c r="A11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="47">
+      <c r="B11" s="50">
         <v>42262</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
       <c r="G11" s="9"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -4988,33 +5351,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
+      <c r="A2" s="58"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="55"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
+      <c r="A3" s="58"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="26"/>
@@ -5038,15 +5401,15 @@
       <c r="F6" s="27"/>
     </row>
     <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="54"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
     </row>
     <row r="8" spans="1:15" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
@@ -5114,24 +5477,24 @@
         <v>245</v>
       </c>
       <c r="C10" s="31">
+        <f>Patients!B77</f>
+        <v>16</v>
+      </c>
+      <c r="D10" s="31">
+        <f>Patients!B73</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="31">
+        <f>Patients!B74</f>
+        <v>2</v>
+      </c>
+      <c r="F10" s="31">
+        <f>Patients!B75</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="31">
         <f>Patients!B76</f>
-        <v>10</v>
-      </c>
-      <c r="D10" s="31">
-        <f>Patients!B72</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="31">
-        <f>Patients!B73</f>
-        <v>2</v>
-      </c>
-      <c r="F10" s="31">
-        <f>Patients!B74</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="31">
-        <f>Patients!B75</f>
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5144,13 +5507,13 @@
       <c r="G11" s="31"/>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="52"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="33">
         <f>SUM(C9:C11)</f>
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D12" s="34">
         <f>SUM(D9:D11)</f>
@@ -5166,7 +5529,7 @@
       </c>
       <c r="G12" s="34">
         <f>SUM(G9:G11)</f>
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5390,18 +5753,18 @@
       <c r="T1" s="3"/>
     </row>
     <row r="2" spans="1:28" s="24" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="59" t="s">
         <v>196</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -5550,18 +5913,18 @@
       <c r="T6" s="3"/>
     </row>
     <row r="7" spans="1:28" s="19" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
@@ -5836,18 +6199,18 @@
       <c r="AB14" s="12"/>
     </row>
     <row r="15" spans="1:28" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
     </row>
     <row r="16" spans="1:28" s="24" customFormat="1" ht="45.6" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
@@ -6202,18 +6565,18 @@
       <c r="J28" s="13"/>
     </row>
     <row r="29" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="56" t="s">
+      <c r="A29" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="B29" s="56"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="56"/>
-      <c r="I29" s="56"/>
-      <c r="J29" s="56"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="59"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="59"/>
+      <c r="J29" s="59"/>
     </row>
     <row r="30" spans="1:20" ht="34.200000000000003" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
@@ -6866,10 +7229,10 @@
       <c r="J56" s="13"/>
     </row>
     <row r="62" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="57" t="s">
+      <c r="A62" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="B62" s="58"/>
+      <c r="B62" s="61"/>
     </row>
     <row r="63" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
@@ -6925,42 +7288,42 @@
     <mergeCell ref="A29:J29"/>
   </mergeCells>
   <conditionalFormatting sqref="G8:G14 G16:G28 G3:G6 G30:G56">
-    <cfRule type="cellIs" dxfId="71" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="17" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:G14 G16:G28 G3:G6 G30:G56">
-    <cfRule type="cellIs" dxfId="70" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="18" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:G14 G16:G28 G3:G6 G30:G56">
-    <cfRule type="cellIs" dxfId="69" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="19" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:G14 G16:G28 G3:G6 G30:G56">
-    <cfRule type="cellIs" dxfId="68" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="20" operator="equal">
       <formula>"Functionality not developed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65">
-    <cfRule type="cellIs" dxfId="67" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="4" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65">
-    <cfRule type="cellIs" dxfId="66" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65">
-    <cfRule type="cellIs" dxfId="65" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65">
-    <cfRule type="cellIs" dxfId="64" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="1" operator="equal">
       <formula>"Functionality not developed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6977,11 +7340,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB76"/>
+  <dimension ref="A1:AB77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7042,18 +7405,18 @@
       <c r="T1" s="3"/>
     </row>
     <row r="2" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="59" t="s">
         <v>196</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -7196,18 +7559,18 @@
       <c r="T7" s="3"/>
     </row>
     <row r="8" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -7384,18 +7747,18 @@
       <c r="T14" s="3"/>
     </row>
     <row r="15" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
     </row>
     <row r="16" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
@@ -7702,18 +8065,18 @@
       <c r="J28" s="13"/>
     </row>
     <row r="29" spans="1:28" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A29" s="56" t="s">
+      <c r="A29" s="59" t="s">
         <v>257</v>
       </c>
-      <c r="B29" s="56"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="56"/>
-      <c r="I29" s="56"/>
-      <c r="J29" s="56"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="59"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="59"/>
+      <c r="J29" s="59"/>
     </row>
     <row r="30" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
@@ -7856,24 +8219,24 @@
       <c r="J39" s="13"/>
     </row>
     <row r="40" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A40" s="56" t="s">
+      <c r="A40" s="59" t="s">
         <v>304</v>
       </c>
-      <c r="B40" s="56"/>
-      <c r="C40" s="56"/>
-      <c r="D40" s="56"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="56"/>
-      <c r="G40" s="56"/>
-      <c r="H40" s="56"/>
-      <c r="I40" s="56"/>
-      <c r="J40" s="56"/>
-    </row>
-    <row r="41" spans="1:11" s="59" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.25">
+      <c r="B40" s="59"/>
+      <c r="C40" s="59"/>
+      <c r="D40" s="59"/>
+      <c r="E40" s="59"/>
+      <c r="F40" s="59"/>
+      <c r="G40" s="59"/>
+      <c r="H40" s="59"/>
+      <c r="I40" s="59"/>
+      <c r="J40" s="59"/>
+    </row>
+    <row r="41" spans="1:11" s="40" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
         <v>283</v>
       </c>
-      <c r="B41" s="61" t="s">
+      <c r="B41" s="42" t="s">
         <v>314</v>
       </c>
       <c r="C41" s="23" t="s">
@@ -7892,14 +8255,14 @@
       <c r="H41" s="13"/>
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
-      <c r="K41" s="60"/>
-    </row>
-    <row r="42" spans="1:11" s="59" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.25">
+      <c r="K41" s="41"/>
+    </row>
+    <row r="42" spans="1:11" s="40" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="B42" s="61" t="s">
-        <v>332</v>
+      <c r="B42" s="42" t="s">
+        <v>326</v>
       </c>
       <c r="C42" s="23" t="s">
         <v>306</v>
@@ -7909,7 +8272,7 @@
       </c>
       <c r="E42" s="23"/>
       <c r="F42" s="23" t="s">
-        <v>318</v>
+        <v>342</v>
       </c>
       <c r="G42" s="21" t="s">
         <v>11</v>
@@ -7919,24 +8282,24 @@
       </c>
       <c r="I42" s="13"/>
       <c r="J42" s="13"/>
-      <c r="K42" s="60"/>
-    </row>
-    <row r="43" spans="1:11" s="59" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.25">
+      <c r="K42" s="41"/>
+    </row>
+    <row r="43" spans="1:11" s="40" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
         <v>285</v>
       </c>
-      <c r="B43" s="61" t="s">
-        <v>319</v>
+      <c r="B43" s="42" t="s">
+        <v>318</v>
       </c>
       <c r="C43" s="23" t="s">
         <v>306</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E43" s="23"/>
       <c r="F43" s="23" t="s">
-        <v>321</v>
+        <v>343</v>
       </c>
       <c r="G43" s="21" t="s">
         <v>12</v>
@@ -7944,24 +8307,24 @@
       <c r="H43" s="13"/>
       <c r="I43" s="13"/>
       <c r="J43" s="13"/>
-      <c r="K43" s="60"/>
-    </row>
-    <row r="44" spans="1:11" s="59" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.25">
+      <c r="K43" s="41"/>
+    </row>
+    <row r="44" spans="1:11" s="40" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
         <v>286</v>
       </c>
-      <c r="B44" s="61" t="s">
-        <v>322</v>
+      <c r="B44" s="42" t="s">
+        <v>320</v>
       </c>
       <c r="C44" s="23" t="s">
         <v>306</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E44" s="23"/>
       <c r="F44" s="23" t="s">
-        <v>324</v>
+        <v>344</v>
       </c>
       <c r="G44" s="21" t="s">
         <v>12</v>
@@ -7969,24 +8332,24 @@
       <c r="H44" s="13"/>
       <c r="I44" s="13"/>
       <c r="J44" s="13"/>
-      <c r="K44" s="60"/>
+      <c r="K44" s="41"/>
     </row>
     <row r="45" spans="1:11" ht="68.400000000000006" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
         <v>287</v>
       </c>
-      <c r="B45" s="61" t="s">
-        <v>325</v>
+      <c r="B45" s="42" t="s">
+        <v>322</v>
       </c>
       <c r="C45" s="23" t="s">
         <v>306</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E45" s="23"/>
       <c r="F45" s="23" t="s">
-        <v>327</v>
+        <v>345</v>
       </c>
       <c r="G45" s="21" t="s">
         <v>12</v>
@@ -7999,18 +8362,18 @@
       <c r="A46" s="20" t="s">
         <v>288</v>
       </c>
-      <c r="B46" s="61" t="s">
-        <v>328</v>
+      <c r="B46" s="42" t="s">
+        <v>324</v>
       </c>
       <c r="C46" s="23" t="s">
         <v>306</v>
       </c>
       <c r="D46" s="23" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="E46" s="23"/>
       <c r="F46" s="23" t="s">
-        <v>330</v>
+        <v>346</v>
       </c>
       <c r="G46" s="21" t="s">
         <v>12</v>
@@ -8024,17 +8387,17 @@
         <v>289</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="C47" s="23" t="s">
         <v>306</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="E47" s="23"/>
       <c r="F47" s="23" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="G47" s="21" t="s">
         <v>11</v>
@@ -8045,72 +8408,122 @@
       <c r="I47" s="13"/>
       <c r="J47" s="13"/>
     </row>
-    <row r="48" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="68.400000000000006" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
         <v>290</v>
       </c>
-      <c r="B48" s="23"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="23"/>
+      <c r="B48" s="23" t="s">
+        <v>340</v>
+      </c>
+      <c r="C48" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="D48" s="23" t="s">
+        <v>337</v>
+      </c>
       <c r="E48" s="23"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="21"/>
+      <c r="F48" s="23" t="s">
+        <v>351</v>
+      </c>
+      <c r="G48" s="21" t="s">
+        <v>12</v>
+      </c>
       <c r="H48" s="13"/>
       <c r="I48" s="13"/>
       <c r="J48" s="13"/>
     </row>
-    <row r="49" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="68.400000000000006" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
         <v>291</v>
       </c>
-      <c r="B49" s="23"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="23"/>
+      <c r="B49" s="23" t="s">
+        <v>339</v>
+      </c>
+      <c r="C49" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="D49" s="23" t="s">
+        <v>341</v>
+      </c>
       <c r="E49" s="23"/>
-      <c r="F49" s="23"/>
-      <c r="G49" s="21"/>
+      <c r="F49" s="23" t="s">
+        <v>350</v>
+      </c>
+      <c r="G49" s="21" t="s">
+        <v>12</v>
+      </c>
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
       <c r="J49" s="13"/>
     </row>
-    <row r="50" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="68.400000000000006" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
         <v>292</v>
       </c>
-      <c r="B50" s="23"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="23"/>
+      <c r="B50" s="23" t="s">
+        <v>347</v>
+      </c>
+      <c r="C50" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="D50" s="23" t="s">
+        <v>348</v>
+      </c>
       <c r="E50" s="23"/>
-      <c r="F50" s="23"/>
-      <c r="G50" s="21"/>
+      <c r="F50" s="23" t="s">
+        <v>349</v>
+      </c>
+      <c r="G50" s="21" t="s">
+        <v>12</v>
+      </c>
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
       <c r="J50" s="13"/>
     </row>
-    <row r="51" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="68.400000000000006" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
         <v>293</v>
       </c>
-      <c r="B51" s="23"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="23"/>
+      <c r="B51" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="C51" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="D51" s="23" t="s">
+        <v>353</v>
+      </c>
       <c r="E51" s="23"/>
-      <c r="F51" s="23"/>
-      <c r="G51" s="21"/>
+      <c r="F51" s="23" t="s">
+        <v>354</v>
+      </c>
+      <c r="G51" s="21" t="s">
+        <v>12</v>
+      </c>
       <c r="H51" s="13"/>
       <c r="I51" s="13"/>
       <c r="J51" s="13"/>
     </row>
-    <row r="52" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="68.400000000000006" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
         <v>294</v>
       </c>
-      <c r="B52" s="23"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="23"/>
+      <c r="B52" s="23" t="s">
+        <v>356</v>
+      </c>
+      <c r="C52" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="D52" s="23" t="s">
+        <v>355</v>
+      </c>
       <c r="E52" s="23"/>
-      <c r="F52" s="23"/>
-      <c r="G52" s="21"/>
+      <c r="F52" s="23" t="s">
+        <v>354</v>
+      </c>
+      <c r="G52" s="21" t="s">
+        <v>12</v>
+      </c>
       <c r="H52" s="13"/>
       <c r="I52" s="13"/>
       <c r="J52" s="13"/>
@@ -8171,37 +8584,47 @@
       <c r="I56" s="13"/>
       <c r="J56" s="13"/>
     </row>
-    <row r="57" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A57" s="20" t="s">
+    <row r="57" spans="1:10" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A57" s="59" t="s">
+        <v>333</v>
+      </c>
+      <c r="B57" s="59"/>
+      <c r="C57" s="59"/>
+      <c r="D57" s="59"/>
+      <c r="E57" s="59"/>
+      <c r="F57" s="59"/>
+      <c r="G57" s="59"/>
+      <c r="H57" s="59"/>
+      <c r="I57" s="59"/>
+      <c r="J57" s="59"/>
+    </row>
+    <row r="58" spans="1:10" ht="79.8" x14ac:dyDescent="0.25">
+      <c r="A58" s="20" t="s">
         <v>299</v>
       </c>
-      <c r="B57" s="23"/>
-      <c r="C57" s="23"/>
-      <c r="D57" s="23"/>
-      <c r="E57" s="23"/>
-      <c r="F57" s="23"/>
-      <c r="G57" s="21"/>
-      <c r="H57" s="13"/>
-      <c r="I57" s="13"/>
-      <c r="J57" s="13"/>
-    </row>
-    <row r="58" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A58" s="20" t="s">
-        <v>300</v>
-      </c>
-      <c r="B58" s="23"/>
-      <c r="C58" s="23"/>
-      <c r="D58" s="23"/>
+      <c r="B58" s="23" t="s">
+        <v>336</v>
+      </c>
+      <c r="C58" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="D58" s="23" t="s">
+        <v>334</v>
+      </c>
       <c r="E58" s="23"/>
-      <c r="F58" s="23"/>
-      <c r="G58" s="21"/>
+      <c r="F58" s="23" t="s">
+        <v>335</v>
+      </c>
+      <c r="G58" s="21" t="s">
+        <v>12</v>
+      </c>
       <c r="H58" s="13"/>
       <c r="I58" s="13"/>
       <c r="J58" s="13"/>
     </row>
     <row r="59" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B59" s="23"/>
       <c r="C59" s="23"/>
@@ -8215,7 +8638,7 @@
     </row>
     <row r="60" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" s="20" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B60" s="23"/>
       <c r="C60" s="23"/>
@@ -8227,9 +8650,9 @@
       <c r="I60" s="13"/>
       <c r="J60" s="13"/>
     </row>
-    <row r="61" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B61" s="23"/>
       <c r="C61" s="23"/>
@@ -8243,7 +8666,7 @@
     </row>
     <row r="62" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="20" t="s">
-        <v>335</v>
+        <v>303</v>
       </c>
       <c r="B62" s="23"/>
       <c r="C62" s="23"/>
@@ -8257,7 +8680,7 @@
     </row>
     <row r="63" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B63" s="23"/>
       <c r="C63" s="23"/>
@@ -8271,7 +8694,7 @@
     </row>
     <row r="64" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="B64" s="23"/>
       <c r="C64" s="23"/>
@@ -8285,7 +8708,7 @@
     </row>
     <row r="65" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="B65" s="23"/>
       <c r="C65" s="23"/>
@@ -8297,273 +8720,425 @@
       <c r="I65" s="13"/>
       <c r="J65" s="13"/>
     </row>
-    <row r="69" spans="1:10" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="57" t="s">
+    <row r="66" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="20" t="s">
+        <v>332</v>
+      </c>
+      <c r="B66" s="23"/>
+      <c r="C66" s="23"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="23"/>
+      <c r="F66" s="23"/>
+      <c r="G66" s="21"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="13"/>
+    </row>
+    <row r="70" spans="1:10" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="B71" s="58"/>
-    </row>
-    <row r="72" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="14" t="s">
+      <c r="B72" s="61"/>
+    </row>
+    <row r="73" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B72" s="15">
-        <f>COUNTIF(G3:G65,"Pass")</f>
+      <c r="B73" s="15">
+        <f>COUNTIF(G3:G66,"Pass")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="6" t="s">
+    <row r="74" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B73" s="5">
-        <f>COUNTIF(G3:G65,"Fail")</f>
+      <c r="B74" s="5">
+        <f>COUNTIF(G3:G66,"Fail")</f>
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="38" t="s">
+    <row r="75" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="B74" s="37">
-        <f>COUNTIF(G3:G65,"Functionality not developed")</f>
+      <c r="B75" s="37">
+        <f>COUNTIF(G3:G66,"Functionality not developed")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="7" t="s">
+    <row r="76" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B75" s="5">
-        <f>COUNTIF(G3:G67,"Not Tested")</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="8" t="s">
+      <c r="B76" s="5">
+        <f>COUNTIF(G3:G68,"Not Tested")</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B76" s="8">
-        <f>SUM(B72:B75)</f>
-        <v>10</v>
+      <c r="B77" s="8">
+        <f>SUM(B73:B76)</f>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A8:J8"/>
     <mergeCell ref="A29:J29"/>
     <mergeCell ref="A15:J15"/>
-    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
     <mergeCell ref="A40:J40"/>
+    <mergeCell ref="A57:J57"/>
   </mergeCells>
-  <conditionalFormatting sqref="A74 G11:G14 G16:G28 G30:G39 G3:G7 G48:G65">
-    <cfRule type="cellIs" dxfId="63" priority="48" operator="equal">
+  <conditionalFormatting sqref="A75 G11:G14 G16:G28 G30:G39 G3:G7 G54:G56 G59:G66">
+    <cfRule type="cellIs" dxfId="95" priority="76" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A74 G11:G14 G16:G28 G30:G39 G3:G7 G48:G65">
-    <cfRule type="cellIs" dxfId="62" priority="47" operator="equal">
+  <conditionalFormatting sqref="A75 G11:G14 G16:G28 G30:G39 G3:G7 G54:G56 G59:G66">
+    <cfRule type="cellIs" dxfId="94" priority="75" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A74 G11:G14 G16:G28 G30:G39 G3:G7 G48:G65">
-    <cfRule type="cellIs" dxfId="61" priority="46" operator="equal">
+  <conditionalFormatting sqref="A75 G11:G14 G16:G28 G30:G39 G3:G7 G54:G56 G59:G66">
+    <cfRule type="cellIs" dxfId="93" priority="74" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A74 G11:G14 G16:G28 G30:G39 G3:G7 G48:G65">
-    <cfRule type="cellIs" dxfId="60" priority="45" operator="equal">
+  <conditionalFormatting sqref="A75 G11:G14 G16:G28 G30:G39 G3:G7 G54:G56 G59:G66">
+    <cfRule type="cellIs" dxfId="92" priority="73" operator="equal">
       <formula>"Functionality not developed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="cellIs" dxfId="59" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="68" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="cellIs" dxfId="58" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="67" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="cellIs" dxfId="57" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="66" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="cellIs" dxfId="56" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="65" operator="equal">
       <formula>"Functionality not developed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G41">
+    <cfRule type="cellIs" dxfId="87" priority="53" operator="equal">
+      <formula>"Functionality not developed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10">
+    <cfRule type="cellIs" dxfId="86" priority="64" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10">
+    <cfRule type="cellIs" dxfId="85" priority="63" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10">
+    <cfRule type="cellIs" dxfId="84" priority="62" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10">
+    <cfRule type="cellIs" dxfId="83" priority="61" operator="equal">
+      <formula>"Functionality not developed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G41">
+    <cfRule type="cellIs" dxfId="82" priority="56" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G41">
+    <cfRule type="cellIs" dxfId="81" priority="55" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G41">
+    <cfRule type="cellIs" dxfId="80" priority="54" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G42">
+    <cfRule type="cellIs" dxfId="79" priority="49" operator="equal">
+      <formula>"Functionality not developed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G42">
+    <cfRule type="cellIs" dxfId="78" priority="52" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G42">
+    <cfRule type="cellIs" dxfId="77" priority="51" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G42">
+    <cfRule type="cellIs" dxfId="76" priority="50" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G43">
+    <cfRule type="cellIs" dxfId="75" priority="45" operator="equal">
+      <formula>"Functionality not developed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G43">
+    <cfRule type="cellIs" dxfId="74" priority="48" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G43">
+    <cfRule type="cellIs" dxfId="73" priority="47" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G43">
+    <cfRule type="cellIs" dxfId="72" priority="46" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G44">
+    <cfRule type="cellIs" dxfId="71" priority="41" operator="equal">
+      <formula>"Functionality not developed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G44">
+    <cfRule type="cellIs" dxfId="70" priority="44" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G44">
+    <cfRule type="cellIs" dxfId="69" priority="43" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G44">
+    <cfRule type="cellIs" dxfId="68" priority="42" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G45">
+    <cfRule type="cellIs" dxfId="67" priority="37" operator="equal">
+      <formula>"Functionality not developed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G45">
+    <cfRule type="cellIs" dxfId="66" priority="40" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G45">
+    <cfRule type="cellIs" dxfId="65" priority="39" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G45">
+    <cfRule type="cellIs" dxfId="64" priority="38" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G46">
+    <cfRule type="cellIs" dxfId="63" priority="33" operator="equal">
+      <formula>"Functionality not developed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G46">
+    <cfRule type="cellIs" dxfId="62" priority="36" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G46">
+    <cfRule type="cellIs" dxfId="61" priority="35" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G46">
+    <cfRule type="cellIs" dxfId="60" priority="34" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G47">
+    <cfRule type="cellIs" dxfId="59" priority="29" operator="equal">
+      <formula>"Functionality not developed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G47">
+    <cfRule type="cellIs" dxfId="58" priority="32" operator="equal">
+      <formula>"Not Tested"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G47">
+    <cfRule type="cellIs" dxfId="57" priority="31" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G47">
+    <cfRule type="cellIs" dxfId="56" priority="30" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G58">
     <cfRule type="cellIs" dxfId="55" priority="25" operator="equal">
       <formula>"Functionality not developed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G10">
-    <cfRule type="cellIs" dxfId="54" priority="36" operator="equal">
+  <conditionalFormatting sqref="G58">
+    <cfRule type="cellIs" dxfId="53" priority="28" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G10">
-    <cfRule type="cellIs" dxfId="53" priority="35" operator="equal">
+  <conditionalFormatting sqref="G58">
+    <cfRule type="cellIs" dxfId="51" priority="27" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G10">
-    <cfRule type="cellIs" dxfId="52" priority="34" operator="equal">
+  <conditionalFormatting sqref="G58">
+    <cfRule type="cellIs" dxfId="49" priority="26" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G10">
-    <cfRule type="cellIs" dxfId="51" priority="33" operator="equal">
-      <formula>"Functionality not developed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G41">
-    <cfRule type="cellIs" dxfId="50" priority="28" operator="equal">
-      <formula>"Not Tested"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G41">
-    <cfRule type="cellIs" dxfId="49" priority="27" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G41">
-    <cfRule type="cellIs" dxfId="48" priority="26" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G42">
+  <conditionalFormatting sqref="G48">
     <cfRule type="cellIs" dxfId="47" priority="21" operator="equal">
       <formula>"Functionality not developed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G42">
+  <conditionalFormatting sqref="G48">
     <cfRule type="cellIs" dxfId="45" priority="24" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G42">
+  <conditionalFormatting sqref="G48">
     <cfRule type="cellIs" dxfId="43" priority="23" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G42">
+  <conditionalFormatting sqref="G48">
     <cfRule type="cellIs" dxfId="41" priority="22" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G43">
+  <conditionalFormatting sqref="G49">
     <cfRule type="cellIs" dxfId="39" priority="17" operator="equal">
       <formula>"Functionality not developed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G43">
+  <conditionalFormatting sqref="G49">
     <cfRule type="cellIs" dxfId="37" priority="20" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G43">
+  <conditionalFormatting sqref="G49">
     <cfRule type="cellIs" dxfId="35" priority="19" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G43">
+  <conditionalFormatting sqref="G49">
     <cfRule type="cellIs" dxfId="33" priority="18" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G44">
+  <conditionalFormatting sqref="G50">
     <cfRule type="cellIs" dxfId="31" priority="13" operator="equal">
       <formula>"Functionality not developed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G44">
+  <conditionalFormatting sqref="G50">
     <cfRule type="cellIs" dxfId="29" priority="16" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G44">
+  <conditionalFormatting sqref="G50">
     <cfRule type="cellIs" dxfId="27" priority="15" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G44">
+  <conditionalFormatting sqref="G50">
     <cfRule type="cellIs" dxfId="25" priority="14" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G45">
+  <conditionalFormatting sqref="G51">
     <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
       <formula>"Functionality not developed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G45">
+  <conditionalFormatting sqref="G51">
     <cfRule type="cellIs" dxfId="21" priority="12" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G45">
+  <conditionalFormatting sqref="G51">
     <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G45">
+  <conditionalFormatting sqref="G51">
     <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G46">
+  <conditionalFormatting sqref="G52">
     <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
       <formula>"Functionality not developed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G46">
+  <conditionalFormatting sqref="G52">
     <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G46">
+  <conditionalFormatting sqref="G52">
     <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G46">
+  <conditionalFormatting sqref="G52">
     <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G47">
+  <conditionalFormatting sqref="G53">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"Functionality not developed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G47">
+  <conditionalFormatting sqref="G53">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G47">
+  <conditionalFormatting sqref="G53">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G47">
+  <conditionalFormatting sqref="G53">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="3">
-    <dataValidation showInputMessage="1" showErrorMessage="1" prompt="Click and Select a value from the list." sqref="A74"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="Click and Select a value from the list." sqref="G16:H28 G11:H14 G30:H39 G3:H7 G9:H9 G41:H65">
-      <formula1>test</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="Click and Select a value from the list." sqref="G10:H10">
+  <dataValidations count="2">
+    <dataValidation showInputMessage="1" showErrorMessage="1" prompt="Click and Select a value from the list." sqref="A75"/>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="Click and Select a value from the list." sqref="G16:H28 G30:H39 G3:H7 G9:H14 G58:H66 G41:H56">
       <formula1>test</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Made Changes in Test_Click_On_Login, etc.
</commit_message>
<xml_diff>
--- a/SocialTables_tBlocks Test cases sheet V1.0.xlsx
+++ b/SocialTables_tBlocks Test cases sheet V1.0.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="168">
   <si>
     <t>Project Name</t>
   </si>
@@ -830,6 +830,12 @@
   </si>
   <si>
     <t>User should able to see the venue and its Property in a new Tab</t>
+  </si>
+  <si>
+    <t>FOOTER (N.A.)</t>
+  </si>
+  <si>
+    <t>TC_PT_35_Chrome.png</t>
   </si>
 </sst>
 </file>
@@ -1361,7 +1367,7 @@
     <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="30" fillId="2" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1512,6 +1518,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5338,7 +5347,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5385,7 +5394,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
@@ -5483,7 +5492,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5498,11 +5507,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1950652096"/>
-        <c:axId val="-1950651008"/>
+        <c:axId val="-1644220160"/>
+        <c:axId val="-1644226688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1950652096"/>
+        <c:axId val="-1644220160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5527,7 +5536,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1950651008"/>
+        <c:crossAx val="-1644226688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -5535,7 +5544,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1950651008"/>
+        <c:axId val="-1644226688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5571,14 +5580,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1950652096"/>
+        <c:crossAx val="-1644220160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -6526,7 +6534,7 @@
       </c>
       <c r="E10" s="28">
         <f>Events!B62</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F10" s="28">
         <f>Homepage!B63</f>
@@ -6559,7 +6567,7 @@
       </c>
       <c r="D12" s="28">
         <f>Events!B62</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E12" s="28">
         <f>Events!B63</f>
@@ -6571,7 +6579,7 @@
       </c>
       <c r="G12" s="28">
         <f>Events!B65</f>
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6631,11 +6639,11 @@
       </c>
       <c r="D16" s="31">
         <f t="shared" ref="D16:G16" si="0">SUM(D10:D15)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E16" s="31">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F16" s="31">
         <f t="shared" si="0"/>
@@ -6643,7 +6651,7 @@
       </c>
       <c r="G16" s="31">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -8314,9 +8322,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8418,9 +8426,11 @@
         <v>39</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="13"/>
+        <v>10</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="I3" s="13"/>
       <c r="J3" s="13"/>
       <c r="K3" s="3"/>
@@ -8434,7 +8444,7 @@
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
     </row>
-    <row r="4" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>40</v>
       </c>
@@ -8458,7 +8468,7 @@
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
     </row>
-    <row r="5" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>41</v>
       </c>
@@ -8482,7 +8492,7 @@
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
     </row>
-    <row r="6" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>42</v>
       </c>
@@ -8506,7 +8516,7 @@
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
     </row>
-    <row r="7" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>43</v>
       </c>
@@ -8572,9 +8582,11 @@
         <v>99</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="13"/>
+        <v>10</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
       <c r="K9" s="3"/>
@@ -8606,9 +8618,11 @@
         <v>95</v>
       </c>
       <c r="G10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="20"/>
       <c r="I10" s="20"/>
       <c r="J10" s="20"/>
       <c r="K10" s="3"/>
@@ -8622,7 +8636,7 @@
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
     </row>
-    <row r="11" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>46</v>
       </c>
@@ -8646,7 +8660,7 @@
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
     </row>
-    <row r="12" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>47</v>
       </c>
@@ -8670,7 +8684,7 @@
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
     </row>
-    <row r="13" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>48</v>
       </c>
@@ -8694,7 +8708,7 @@
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
     </row>
-    <row r="14" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>50</v>
       </c>
@@ -8720,7 +8734,7 @@
     </row>
     <row r="15" spans="1:20" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="s">
-        <v>34</v>
+        <v>166</v>
       </c>
       <c r="B15" s="63"/>
       <c r="C15" s="63"/>
@@ -8756,7 +8770,7 @@
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
     </row>
-    <row r="17" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>52</v>
       </c>
@@ -8788,7 +8802,7 @@
       <c r="AA17" s="12"/>
       <c r="AB17" s="12"/>
     </row>
-    <row r="18" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
         <v>53</v>
       </c>
@@ -8820,7 +8834,7 @@
       <c r="AA18" s="12"/>
       <c r="AB18" s="12"/>
     </row>
-    <row r="19" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
         <v>54</v>
       </c>
@@ -8852,7 +8866,7 @@
       <c r="AA19" s="12"/>
       <c r="AB19" s="12"/>
     </row>
-    <row r="20" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
         <v>55</v>
       </c>
@@ -8884,7 +8898,7 @@
       <c r="AA20" s="12"/>
       <c r="AB20" s="12"/>
     </row>
-    <row r="21" spans="1:28" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
         <v>56</v>
       </c>
@@ -8908,7 +8922,7 @@
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
     </row>
-    <row r="22" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>57</v>
       </c>
@@ -8932,7 +8946,7 @@
       <c r="S22" s="4"/>
       <c r="T22" s="4"/>
     </row>
-    <row r="23" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>58</v>
       </c>
@@ -8998,9 +9012,11 @@
         <v>102</v>
       </c>
       <c r="G25" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="13"/>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
     </row>
@@ -9028,7 +9044,9 @@
         <v>11</v>
       </c>
       <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
+      <c r="J26" s="66" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="27" spans="1:28" ht="68.400000000000006" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
@@ -9579,7 +9597,7 @@
       </c>
       <c r="B62" s="15">
         <f>COUNTIF(G3:G55,"Pass")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9606,7 +9624,7 @@
       </c>
       <c r="B65" s="15">
         <f>COUNTIF(G3:G57,"Not Tested")</f>
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9993,8 +10011,11 @@
       <formula1>test</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="J26" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>